<commit_message>
update experiments, added wrf
</commit_message>
<xml_diff>
--- a/exp_results1.0.xlsx
+++ b/exp_results1.0.xlsx
@@ -107,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -120,7 +120,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -533,7 +532,7 @@
     <col width="25" customWidth="1" min="31" max="31"/>
     <col width="24" customWidth="1" min="32" max="32"/>
     <col width="23" customWidth="1" min="33" max="33"/>
-    <col width="21" customWidth="1" min="34" max="34"/>
+    <col width="23" customWidth="1" min="34" max="34"/>
     <col width="22" customWidth="1" min="35" max="35"/>
     <col width="27" customWidth="1" min="36" max="36"/>
     <col width="26" customWidth="1" min="37" max="37"/>
@@ -769,94 +768,94 @@
         <v>6305.732591307863</v>
       </c>
       <c r="J2" s="6" t="n">
+        <v>7538.57225522959</v>
+      </c>
+      <c r="K2" s="7" t="n">
+        <v>-0.1075154290841148</v>
+      </c>
+      <c r="L2" s="8" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="M2" s="8" t="n">
+        <v>13088.07342086904</v>
+      </c>
+      <c r="N2" s="8" t="n">
+        <v>8175.901165639443</v>
+      </c>
+      <c r="O2" s="6" t="n">
+        <v>6919.371499910049</v>
+      </c>
+      <c r="P2" s="7" t="n">
+        <v>-0.1808220316757115</v>
+      </c>
+      <c r="Q2" s="8" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="R2" s="8" t="n">
+        <v>13145.78078026208</v>
+      </c>
+      <c r="S2" s="8" t="n">
+        <v>8343.209280352034</v>
+      </c>
+      <c r="T2" s="6" t="n">
+        <v>7301.753897251701</v>
+      </c>
+      <c r="U2" s="7" t="n">
+        <v>-0.1355521346364534</v>
+      </c>
+      <c r="V2" s="8" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="W2" s="8" t="n">
+        <v>12990.9715051854</v>
+      </c>
+      <c r="X2" s="8" t="n">
+        <v>7962.817607933697</v>
+      </c>
+      <c r="Y2" s="4" t="n">
+        <v>1.653151750564575</v>
+      </c>
+      <c r="Z2" s="4" t="n">
+        <v>0.02076601982116699</v>
+      </c>
+      <c r="AA2" s="4" t="n">
+        <v>1.673917770385742</v>
+      </c>
+      <c r="AB2" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L2" s="8" t="n">
+      <c r="AC2" s="9" t="n">
+        <v>6.365776062011719e-05</v>
+      </c>
+      <c r="AD2" s="9" t="n">
+        <v>6.365776062011719e-05</v>
+      </c>
+      <c r="AE2" s="10" t="n">
+        <v>26295.58052434457</v>
+      </c>
+      <c r="AF2" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="6" t="n">
-        <v>7299.872538061414</v>
-      </c>
-      <c r="U2" s="7" t="n">
-        <v>-0.1357748670044449</v>
-      </c>
-      <c r="V2" s="9" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="W2" s="9" t="n">
-        <v>13008.40404399576</v>
-      </c>
-      <c r="X2" s="9" t="n">
-        <v>7942.931505934343</v>
-      </c>
-      <c r="Y2" s="4" t="n">
-        <v>1.7019362449646</v>
-      </c>
-      <c r="Z2" s="4" t="n">
-        <v>0.02213525772094727</v>
-      </c>
-      <c r="AA2" s="4" t="n">
-        <v>1.724071502685547</v>
-      </c>
-      <c r="AB2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="10" t="n">
-        <v>0.001309394836425781</v>
-      </c>
-      <c r="AK2" s="10" t="n">
-        <v>4.982948303222656e-05</v>
-      </c>
-      <c r="AL2" s="10" t="n">
-        <v>0.001359224319458008</v>
-      </c>
-      <c r="AM2" s="11" t="n">
-        <v>1268.423083669532</v>
+      <c r="AG2" s="9" t="n">
+        <v>1.33514404296875e-05</v>
+      </c>
+      <c r="AH2" s="9" t="n">
+        <v>1.33514404296875e-05</v>
+      </c>
+      <c r="AI2" s="10" t="n">
+        <v>125373.5714285714</v>
+      </c>
+      <c r="AJ2" s="9" t="n">
+        <v>0.001269102096557617</v>
+      </c>
+      <c r="AK2" s="9" t="n">
+        <v>4.9591064453125e-05</v>
+      </c>
+      <c r="AL2" s="9" t="n">
+        <v>0.001318693161010742</v>
+      </c>
+      <c r="AM2" s="10" t="n">
+        <v>1269.376242994034</v>
       </c>
     </row>
     <row r="3">
@@ -890,94 +889,94 @@
         <v>6721.42924321072</v>
       </c>
       <c r="J3" s="6" t="n">
+        <v>6437.274477226392</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>-0.1413774391854961</v>
+      </c>
+      <c r="L3" s="8" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <v>13001.68972507055</v>
+      </c>
+      <c r="N3" s="8" t="n">
+        <v>9347.615247844155</v>
+      </c>
+      <c r="O3" s="6" t="n">
+        <v>5690.659344165869</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>-0.2409631566749731</v>
+      </c>
+      <c r="Q3" s="8" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="R3" s="8" t="n">
+        <v>13141.22257621717</v>
+      </c>
+      <c r="S3" s="8" t="n">
+        <v>9684.963232051299</v>
+      </c>
+      <c r="T3" s="6" t="n">
+        <v>6132.510961599255</v>
+      </c>
+      <c r="U3" s="7" t="n">
+        <v>-0.1820276912691002</v>
+      </c>
+      <c r="V3" s="8" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="W3" s="8" t="n">
+        <v>12962.59019297255</v>
+      </c>
+      <c r="X3" s="8" t="n">
+        <v>9103.679231373299</v>
+      </c>
+      <c r="Y3" s="4" t="n">
+        <v>1.631019115447998</v>
+      </c>
+      <c r="Z3" s="4" t="n">
+        <v>0.02161550521850586</v>
+      </c>
+      <c r="AA3" s="4" t="n">
+        <v>1.652634620666504</v>
+      </c>
+      <c r="AB3" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L3" s="8" t="n">
+      <c r="AC3" s="9" t="n">
+        <v>6.270408630371094e-05</v>
+      </c>
+      <c r="AD3" s="9" t="n">
+        <v>6.270408630371094e-05</v>
+      </c>
+      <c r="AE3" s="10" t="n">
+        <v>26356.09125475285</v>
+      </c>
+      <c r="AF3" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="6" t="n">
-        <v>6250.948469929583</v>
-      </c>
-      <c r="U3" s="7" t="n">
-        <v>-0.1662301488373083</v>
-      </c>
-      <c r="V3" s="9" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="W3" s="9" t="n">
-        <v>12955.09027067977</v>
-      </c>
-      <c r="X3" s="9" t="n">
-        <v>9095.34180075018</v>
-      </c>
-      <c r="Y3" s="4" t="n">
-        <v>1.625311613082886</v>
-      </c>
-      <c r="Z3" s="4" t="n">
-        <v>0.02171874046325684</v>
-      </c>
-      <c r="AA3" s="4" t="n">
-        <v>1.647030353546143</v>
-      </c>
-      <c r="AB3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="10" t="n">
-        <v>0.001293659210205078</v>
-      </c>
-      <c r="AK3" s="10" t="n">
-        <v>4.529953002929688e-05</v>
-      </c>
-      <c r="AL3" s="10" t="n">
-        <v>0.001338958740234375</v>
-      </c>
-      <c r="AM3" s="11" t="n">
-        <v>1230.082977207977</v>
+      <c r="AG3" s="9" t="n">
+        <v>1.192092895507812e-05</v>
+      </c>
+      <c r="AH3" s="9" t="n">
+        <v>1.192092895507812e-05</v>
+      </c>
+      <c r="AI3" s="10" t="n">
+        <v>138633.04</v>
+      </c>
+      <c r="AJ3" s="9" t="n">
+        <v>0.001333713531494141</v>
+      </c>
+      <c r="AK3" s="9" t="n">
+        <v>4.839897155761719e-05</v>
+      </c>
+      <c r="AL3" s="9" t="n">
+        <v>0.001382112503051758</v>
+      </c>
+      <c r="AM3" s="10" t="n">
+        <v>1195.730895290668</v>
       </c>
     </row>
     <row r="4">
@@ -1011,94 +1010,94 @@
         <v>8449.266394186443</v>
       </c>
       <c r="J4" s="6" t="n">
+        <v>3164.426659325243</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>-0.4103192028928591</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="M4" s="8" t="n">
+        <v>12647.25672972156</v>
+      </c>
+      <c r="N4" s="8" t="n">
+        <v>11678.03007039631</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>2971.872903799926</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>-0.446200979994419</v>
+      </c>
+      <c r="Q4" s="8" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="R4" s="8" t="n">
+        <v>12955.36841500388</v>
+      </c>
+      <c r="S4" s="8" t="n">
+        <v>12296.29551120396</v>
+      </c>
+      <c r="T4" s="6" t="n">
+        <v>3091.461521747658</v>
+      </c>
+      <c r="U4" s="7" t="n">
+        <v>-0.4239160231449541</v>
+      </c>
+      <c r="V4" s="8" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="W4" s="8" t="n">
+        <v>13009.9407013498</v>
+      </c>
+      <c r="X4" s="8" t="n">
+        <v>12231.27917960214</v>
+      </c>
+      <c r="Y4" s="4" t="n">
+        <v>1.697639465332031</v>
+      </c>
+      <c r="Z4" s="4" t="n">
+        <v>0.02101659774780273</v>
+      </c>
+      <c r="AA4" s="4" t="n">
+        <v>1.718656063079834</v>
+      </c>
+      <c r="AB4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L4" s="8" t="n">
+      <c r="AC4" s="9" t="n">
+        <v>6.866455078125e-05</v>
+      </c>
+      <c r="AD4" s="9" t="n">
+        <v>6.866455078125e-05</v>
+      </c>
+      <c r="AE4" s="10" t="n">
+        <v>25029.74305555555</v>
+      </c>
+      <c r="AF4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6" t="n">
-        <v>2803.498253242126</v>
-      </c>
-      <c r="U4" s="7" t="n">
-        <v>-0.4775770581414572</v>
-      </c>
-      <c r="V4" s="9" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="W4" s="9" t="n">
-        <v>13052.29121913548</v>
-      </c>
-      <c r="X4" s="9" t="n">
-        <v>12365.59296589335</v>
-      </c>
-      <c r="Y4" s="4" t="n">
-        <v>1.657136678695679</v>
-      </c>
-      <c r="Z4" s="4" t="n">
-        <v>0.02035355567932129</v>
-      </c>
-      <c r="AA4" s="4" t="n">
-        <v>1.677490234375</v>
-      </c>
-      <c r="AB4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="10" t="n">
-        <v>0.00129389762878418</v>
-      </c>
-      <c r="AK4" s="10" t="n">
-        <v>5.53131103515625e-05</v>
-      </c>
-      <c r="AL4" s="10" t="n">
-        <v>0.001349210739135742</v>
-      </c>
-      <c r="AM4" s="11" t="n">
-        <v>1243.312245979855</v>
+      <c r="AG4" s="9" t="n">
+        <v>1.502037048339844e-05</v>
+      </c>
+      <c r="AH4" s="9" t="n">
+        <v>1.502037048339844e-05</v>
+      </c>
+      <c r="AI4" s="10" t="n">
+        <v>114421.6825396825</v>
+      </c>
+      <c r="AJ4" s="9" t="n">
+        <v>0.001480579376220703</v>
+      </c>
+      <c r="AK4" s="9" t="n">
+        <v>5.769729614257812e-05</v>
+      </c>
+      <c r="AL4" s="9" t="n">
+        <v>0.001538276672363281</v>
+      </c>
+      <c r="AM4" s="10" t="n">
+        <v>1117.260694358338</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1157,7 @@
     <col width="25" customWidth="1" min="33" max="33"/>
     <col width="24" customWidth="1" min="34" max="34"/>
     <col width="23" customWidth="1" min="35" max="35"/>
-    <col width="21" customWidth="1" min="36" max="36"/>
+    <col width="23" customWidth="1" min="36" max="36"/>
     <col width="22" customWidth="1" min="37" max="37"/>
     <col width="27" customWidth="1" min="38" max="38"/>
     <col width="26" customWidth="1" min="39" max="39"/>
@@ -1412,94 +1411,94 @@
         <v>8449.266394186443</v>
       </c>
       <c r="L2" s="6" t="n">
+        <v>3164.426659325243</v>
+      </c>
+      <c r="M2" s="7" t="n">
+        <v>-0.4103192028928591</v>
+      </c>
+      <c r="N2" s="8" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="O2" s="8" t="n">
+        <v>12647.25672972156</v>
+      </c>
+      <c r="P2" s="8" t="n">
+        <v>11678.03007039631</v>
+      </c>
+      <c r="Q2" s="6" t="n">
+        <v>2971.872903799926</v>
+      </c>
+      <c r="R2" s="7" t="n">
+        <v>-0.446200979994419</v>
+      </c>
+      <c r="S2" s="8" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="T2" s="8" t="n">
+        <v>12955.36841500388</v>
+      </c>
+      <c r="U2" s="8" t="n">
+        <v>12296.29551120396</v>
+      </c>
+      <c r="V2" s="6" t="n">
+        <v>3091.461521747658</v>
+      </c>
+      <c r="W2" s="7" t="n">
+        <v>-0.4239160231449541</v>
+      </c>
+      <c r="X2" s="8" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="Y2" s="8" t="n">
+        <v>13009.9407013498</v>
+      </c>
+      <c r="Z2" s="8" t="n">
+        <v>12231.27917960214</v>
+      </c>
+      <c r="AA2" s="4" t="n">
+        <v>1.697639465332031</v>
+      </c>
+      <c r="AB2" s="4" t="n">
+        <v>0.02101659774780273</v>
+      </c>
+      <c r="AC2" s="4" t="n">
+        <v>1.718656063079834</v>
+      </c>
+      <c r="AD2" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N2" s="8" t="n">
+      <c r="AE2" s="9" t="n">
+        <v>6.866455078125e-05</v>
+      </c>
+      <c r="AF2" s="9" t="n">
+        <v>6.866455078125e-05</v>
+      </c>
+      <c r="AG2" s="10" t="n">
+        <v>25029.74305555555</v>
+      </c>
+      <c r="AH2" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="S2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" s="6" t="n">
-        <v>2803.498253242126</v>
-      </c>
-      <c r="W2" s="7" t="n">
-        <v>-0.4775770581414572</v>
-      </c>
-      <c r="X2" s="9" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="Y2" s="9" t="n">
-        <v>13052.29121913548</v>
-      </c>
-      <c r="Z2" s="9" t="n">
-        <v>12365.59296589335</v>
-      </c>
-      <c r="AA2" s="4" t="n">
-        <v>1.657136678695679</v>
-      </c>
-      <c r="AB2" s="4" t="n">
-        <v>0.02035355567932129</v>
-      </c>
-      <c r="AC2" s="4" t="n">
-        <v>1.677490234375</v>
-      </c>
-      <c r="AD2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="10" t="n">
-        <v>0.00129389762878418</v>
-      </c>
-      <c r="AM2" s="10" t="n">
-        <v>5.53131103515625e-05</v>
-      </c>
-      <c r="AN2" s="10" t="n">
-        <v>0.001349210739135742</v>
-      </c>
-      <c r="AO2" s="11" t="n">
-        <v>1243.312245979855</v>
+      <c r="AI2" s="9" t="n">
+        <v>1.502037048339844e-05</v>
+      </c>
+      <c r="AJ2" s="9" t="n">
+        <v>1.502037048339844e-05</v>
+      </c>
+      <c r="AK2" s="10" t="n">
+        <v>114421.6825396825</v>
+      </c>
+      <c r="AL2" s="9" t="n">
+        <v>0.001480579376220703</v>
+      </c>
+      <c r="AM2" s="9" t="n">
+        <v>5.769729614257812e-05</v>
+      </c>
+      <c r="AN2" s="9" t="n">
+        <v>0.001538276672363281</v>
+      </c>
+      <c r="AO2" s="10" t="n">
+        <v>1117.260694358338</v>
       </c>
     </row>
     <row r="3">
@@ -1541,94 +1540,94 @@
         <v>6305.732591307863</v>
       </c>
       <c r="L3" s="6" t="n">
+        <v>7538.57225522959</v>
+      </c>
+      <c r="M3" s="7" t="n">
+        <v>-0.1075154290841148</v>
+      </c>
+      <c r="N3" s="8" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="O3" s="8" t="n">
+        <v>13088.07342086904</v>
+      </c>
+      <c r="P3" s="8" t="n">
+        <v>8175.901165639443</v>
+      </c>
+      <c r="Q3" s="6" t="n">
+        <v>6919.371499910049</v>
+      </c>
+      <c r="R3" s="7" t="n">
+        <v>-0.1808220316757115</v>
+      </c>
+      <c r="S3" s="8" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="T3" s="8" t="n">
+        <v>13145.78078026208</v>
+      </c>
+      <c r="U3" s="8" t="n">
+        <v>8343.209280352034</v>
+      </c>
+      <c r="V3" s="6" t="n">
+        <v>7301.753897251701</v>
+      </c>
+      <c r="W3" s="7" t="n">
+        <v>-0.1355521346364534</v>
+      </c>
+      <c r="X3" s="8" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="Y3" s="8" t="n">
+        <v>12990.9715051854</v>
+      </c>
+      <c r="Z3" s="8" t="n">
+        <v>7962.817607933697</v>
+      </c>
+      <c r="AA3" s="4" t="n">
+        <v>1.653151750564575</v>
+      </c>
+      <c r="AB3" s="4" t="n">
+        <v>0.02076601982116699</v>
+      </c>
+      <c r="AC3" s="4" t="n">
+        <v>1.673917770385742</v>
+      </c>
+      <c r="AD3" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N3" s="8" t="n">
+      <c r="AE3" s="9" t="n">
+        <v>6.365776062011719e-05</v>
+      </c>
+      <c r="AF3" s="9" t="n">
+        <v>6.365776062011719e-05</v>
+      </c>
+      <c r="AG3" s="10" t="n">
+        <v>26295.58052434457</v>
+      </c>
+      <c r="AH3" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="S3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" s="6" t="n">
-        <v>7299.872538061414</v>
-      </c>
-      <c r="W3" s="7" t="n">
-        <v>-0.1357748670044449</v>
-      </c>
-      <c r="X3" s="9" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="Y3" s="9" t="n">
-        <v>13008.40404399576</v>
-      </c>
-      <c r="Z3" s="9" t="n">
-        <v>7942.931505934343</v>
-      </c>
-      <c r="AA3" s="4" t="n">
-        <v>1.7019362449646</v>
-      </c>
-      <c r="AB3" s="4" t="n">
-        <v>0.02213525772094727</v>
-      </c>
-      <c r="AC3" s="4" t="n">
-        <v>1.724071502685547</v>
-      </c>
-      <c r="AD3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="10" t="n">
-        <v>0.001309394836425781</v>
-      </c>
-      <c r="AM3" s="10" t="n">
-        <v>4.982948303222656e-05</v>
-      </c>
-      <c r="AN3" s="10" t="n">
-        <v>0.001359224319458008</v>
-      </c>
-      <c r="AO3" s="11" t="n">
-        <v>1268.423083669532</v>
+      <c r="AI3" s="9" t="n">
+        <v>1.33514404296875e-05</v>
+      </c>
+      <c r="AJ3" s="9" t="n">
+        <v>1.33514404296875e-05</v>
+      </c>
+      <c r="AK3" s="10" t="n">
+        <v>125373.5714285714</v>
+      </c>
+      <c r="AL3" s="9" t="n">
+        <v>0.001269102096557617</v>
+      </c>
+      <c r="AM3" s="9" t="n">
+        <v>4.9591064453125e-05</v>
+      </c>
+      <c r="AN3" s="9" t="n">
+        <v>0.001318693161010742</v>
+      </c>
+      <c r="AO3" s="10" t="n">
+        <v>1269.376242994034</v>
       </c>
     </row>
     <row r="4">
@@ -1670,94 +1669,94 @@
         <v>6721.42924321072</v>
       </c>
       <c r="L4" s="6" t="n">
+        <v>6437.274477226392</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <v>-0.1413774391854961</v>
+      </c>
+      <c r="N4" s="8" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="O4" s="8" t="n">
+        <v>13001.68972507055</v>
+      </c>
+      <c r="P4" s="8" t="n">
+        <v>9347.615247844155</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>5690.659344165869</v>
+      </c>
+      <c r="R4" s="7" t="n">
+        <v>-0.2409631566749731</v>
+      </c>
+      <c r="S4" s="8" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="T4" s="8" t="n">
+        <v>13141.22257621717</v>
+      </c>
+      <c r="U4" s="8" t="n">
+        <v>9684.963232051299</v>
+      </c>
+      <c r="V4" s="6" t="n">
+        <v>6132.510961599255</v>
+      </c>
+      <c r="W4" s="7" t="n">
+        <v>-0.1820276912691002</v>
+      </c>
+      <c r="X4" s="8" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="Y4" s="8" t="n">
+        <v>12962.59019297255</v>
+      </c>
+      <c r="Z4" s="8" t="n">
+        <v>9103.679231373299</v>
+      </c>
+      <c r="AA4" s="4" t="n">
+        <v>1.631019115447998</v>
+      </c>
+      <c r="AB4" s="4" t="n">
+        <v>0.02161550521850586</v>
+      </c>
+      <c r="AC4" s="4" t="n">
+        <v>1.652634620666504</v>
+      </c>
+      <c r="AD4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N4" s="8" t="n">
+      <c r="AE4" s="9" t="n">
+        <v>6.270408630371094e-05</v>
+      </c>
+      <c r="AF4" s="9" t="n">
+        <v>6.270408630371094e-05</v>
+      </c>
+      <c r="AG4" s="10" t="n">
+        <v>26356.09125475285</v>
+      </c>
+      <c r="AH4" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="O4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="S4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" s="6" t="n">
-        <v>6250.948469929583</v>
-      </c>
-      <c r="W4" s="7" t="n">
-        <v>-0.1662301488373083</v>
-      </c>
-      <c r="X4" s="9" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="Y4" s="9" t="n">
-        <v>12955.09027067977</v>
-      </c>
-      <c r="Z4" s="9" t="n">
-        <v>9095.34180075018</v>
-      </c>
-      <c r="AA4" s="4" t="n">
-        <v>1.625311613082886</v>
-      </c>
-      <c r="AB4" s="4" t="n">
-        <v>0.02171874046325684</v>
-      </c>
-      <c r="AC4" s="4" t="n">
-        <v>1.647030353546143</v>
-      </c>
-      <c r="AD4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="10" t="n">
-        <v>0.001293659210205078</v>
-      </c>
-      <c r="AM4" s="10" t="n">
-        <v>4.529953002929688e-05</v>
-      </c>
-      <c r="AN4" s="10" t="n">
-        <v>0.001338958740234375</v>
-      </c>
-      <c r="AO4" s="11" t="n">
-        <v>1230.082977207977</v>
+      <c r="AI4" s="9" t="n">
+        <v>1.192092895507812e-05</v>
+      </c>
+      <c r="AJ4" s="9" t="n">
+        <v>1.192092895507812e-05</v>
+      </c>
+      <c r="AK4" s="10" t="n">
+        <v>138633.04</v>
+      </c>
+      <c r="AL4" s="9" t="n">
+        <v>0.001333713531494141</v>
+      </c>
+      <c r="AM4" s="9" t="n">
+        <v>4.839897155761719e-05</v>
+      </c>
+      <c r="AN4" s="9" t="n">
+        <v>0.001382112503051758</v>
+      </c>
+      <c r="AO4" s="10" t="n">
+        <v>1195.730895290668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>